<commit_message>
[java] ... [core] framework improved:
- workbook reader implementedi: CalcTableWorkbookDataReader
- sheet readers hierarchy optimized/unified: CalcTableSheetDataReader
- core test cases extended with some for:
  - comment-cells within the structure description area
  - different amount of collection elements within the data records
- the bug throwed an Exception by non-existent cells within the getCell(..) fixed
</commit_message>
<xml_diff>
--- a/java/core/src/test/resources/UnitTest_CalcTable_Landscape_DataParser.xlsx
+++ b/java/core/src/test/resources/UnitTest_CalcTable_Landscape_DataParser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19695" windowHeight="10485" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="19695" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UT - Data Primitive Types" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>bool</t>
   </si>
@@ -476,42 +476,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,6 +485,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -858,34 +858,34 @@
   <sheetData>
     <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="12"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="16"/>
       <c r="V2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1037,13 +1037,13 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="14" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -1055,24 +1055,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="26">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1136,27 +1136,69 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="7" t="s">
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" s="8"/>
@@ -1209,114 +1251,114 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="11" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[java] ... framework improved: - workbook reader implemented (CalcTableWorkbookDataReader) - sheet readers hierarchy optimized/unified (CalcTableSheetDataReader) - core test cases extended with some:   - for comment-cells within the structure description area   - for different count of collection elements within the data records - the bug by non-existent Cells (throwing Exception by getCell(..)) fixed
</commit_message>
<xml_diff>
--- a/java/core/src/test/resources/UnitTest_CalcTable_Landscape_DataParser.xlsx
+++ b/java/core/src/test/resources/UnitTest_CalcTable_Landscape_DataParser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19695" windowHeight="10485" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="19695" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UT - Data Primitive Types" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>bool</t>
   </si>
@@ -476,42 +476,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,6 +485,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -858,34 +858,34 @@
   <sheetData>
     <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="12"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="16"/>
       <c r="V2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1037,13 +1037,13 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="14" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -1055,24 +1055,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="26">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1136,27 +1136,69 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="7" t="s">
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" s="8"/>
@@ -1209,114 +1251,114 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="11" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>